<commit_message>
membuat dashboard dan perubahan penempatan untuk uplaod file
</commit_message>
<xml_diff>
--- a/public/excel/dataTraning1.xlsx
+++ b/public/excel/dataTraning1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pekerjaan\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E7AF1-F5D3-45C9-9826-A454C7332A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BE31A9-1BDF-4B9D-AF32-9A37733E4ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{728DBF00-686C-41CD-B2A9-0209504A1EC3}"/>
   </bookViews>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,7 +196,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,14 +513,14 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="6" customWidth="1"/>
     <col min="2" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" style="8" customWidth="1"/>
@@ -662,7 +661,7 @@
         <v>140000</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ref="H3:H11" si="0">F5*G5</f>
+        <f t="shared" ref="H5:H11" si="0">F5*G5</f>
         <v>280000</v>
       </c>
     </row>
@@ -705,7 +704,7 @@
       <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4">
@@ -733,7 +732,7 @@
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4">

</xml_diff>

<commit_message>
firman push yang ke-2
</commit_message>
<xml_diff>
--- a/public/excel/dataTraning1.xlsx
+++ b/public/excel/dataTraning1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pekerjaan\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E7AF1-F5D3-45C9-9826-A454C7332A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BE31A9-1BDF-4B9D-AF32-9A37733E4ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{728DBF00-686C-41CD-B2A9-0209504A1EC3}"/>
   </bookViews>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,7 +196,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,14 +513,14 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="6" customWidth="1"/>
     <col min="2" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" style="8" customWidth="1"/>
@@ -662,7 +661,7 @@
         <v>140000</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ref="H3:H11" si="0">F5*G5</f>
+        <f t="shared" ref="H5:H11" si="0">F5*G5</f>
         <v>280000</v>
       </c>
     </row>
@@ -705,7 +704,7 @@
       <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4">
@@ -733,7 +732,7 @@
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4">

</xml_diff>